<commit_message>
Add product value column to admin table; update script references and implement theme control in adm.js
</commit_message>
<xml_diff>
--- a/Public/produtos.xlsx
+++ b/Public/produtos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kleber\OneDrive\Documentos\Repositorios\Nelson\Platotruck\Public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9343268-A26C-4D6D-A554-FF5E63F2B351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89487F6-203A-4746-973F-B348AD47622D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FF681648-D961-4BB7-BB4E-8A970B45B2B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FF681648-D961-4BB7-BB4E-8A970B45B2B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Base_vendas" sheetId="1" r:id="rId1"/>
@@ -2396,15 +2396,16 @@
     <t>Marca</t>
   </si>
   <si>
-    <t>VALOR</t>
+    <t>Valor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -2470,7 +2471,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -2813,7 +2814,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>

</xml_diff>